<commit_message>
added the DataGridX class to calculate dimensions.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>Progress</t>
   </si>
@@ -41,27 +41,15 @@
     <t>Displays tabular data.</t>
   </si>
   <si>
-    <t>Input Value</t>
-  </si>
-  <si>
     <t>Reads a value from the user.</t>
   </si>
   <si>
-    <t>Input List of Values</t>
-  </si>
-  <si>
     <t>Reads a list of values of the same type from the user.</t>
   </si>
   <si>
-    <t>Output Value</t>
-  </si>
-  <si>
     <t>Displays a value to the user.</t>
   </si>
   <si>
-    <t>Output List of Values</t>
-  </si>
-  <si>
     <t>Displays a list of values to the user.</t>
   </si>
   <si>
@@ -152,9 +140,6 @@
     <t>Done()</t>
   </si>
   <si>
-    <t>Start()</t>
-  </si>
-  <si>
     <t>Stop()</t>
   </si>
   <si>
@@ -182,15 +167,9 @@
     <t>Quick Method</t>
   </si>
   <si>
-    <t>TextInput</t>
-  </si>
-  <si>
     <t>ListInput</t>
   </si>
   <si>
-    <t>TextOutput</t>
-  </si>
-  <si>
     <t>OutputList</t>
   </si>
   <si>
@@ -263,15 +242,6 @@
     <t>Dispose Method</t>
   </si>
   <si>
-    <t>DataRow</t>
-  </si>
-  <si>
-    <t>DataDolumn</t>
-  </si>
-  <si>
-    <t>DataCell</t>
-  </si>
-  <si>
     <t>???</t>
   </si>
   <si>
@@ -279,6 +249,48 @@
   </si>
   <si>
     <t>Render()</t>
+  </si>
+  <si>
+    <t>ValueInput</t>
+  </si>
+  <si>
+    <t>ValueOutput</t>
+  </si>
+  <si>
+    <t>Read Value</t>
+  </si>
+  <si>
+    <t>Read List of Values</t>
+  </si>
+  <si>
+    <t>Display Value</t>
+  </si>
+  <si>
+    <t>Display List of Values</t>
+  </si>
+  <si>
+    <t>Table / DataGrid</t>
+  </si>
+  <si>
+    <t>Column / DataGridColumn</t>
+  </si>
+  <si>
+    <t>DataRow / DataGridRow</t>
+  </si>
+  <si>
+    <t>DataCell / DataGridCell</t>
+  </si>
+  <si>
+    <t>ColumnList / DataGridHeaderRow</t>
+  </si>
+  <si>
+    <t>ColumnCell / DataGridColumnHeaderCell</t>
+  </si>
+  <si>
+    <t>TitleRow / DataGridTitleRow</t>
+  </si>
+  <si>
+    <t>TitleCell / DataGridTitleCell</t>
   </si>
 </sst>
 </file>
@@ -684,17 +696,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
@@ -702,27 +717,27 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -733,21 +748,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -757,7 +772,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -767,7 +782,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -776,377 +791,417 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" t="s">
-        <v>35</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
+      <c r="C8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" t="s">
-        <v>35</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" t="s">
-        <v>46</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
+      <c r="C10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
         <v>42</v>
       </c>
-      <c r="E17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
+    </row>
+    <row r="17" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
         <v>70</v>
       </c>
-      <c r="H17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="1"/>
-      <c r="H19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
       <c r="H21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" t="s">
-        <v>68</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="1"/>
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
         <v>60</v>
       </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="1"/>
-      <c r="G24" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" t="s">
+        <v>61</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" t="s">
-        <v>82</v>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added quick method for the YesNoQuestion. renamed the IsSelectable property into IsEnabled in menu item.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
   <si>
     <t>Progress</t>
   </si>
@@ -182,9 +182,6 @@
     <t>ProgressBar</t>
   </si>
   <si>
-    <t>SelectableMenu</t>
-  </si>
-  <si>
     <t>MachineLevelGuardian</t>
   </si>
   <si>
@@ -291,6 +288,9 @@
   </si>
   <si>
     <t>TitleCell / DataGridTitleCell</t>
+  </si>
+  <si>
+    <t>ScrollableMenu</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +729,7 @@
         <v>46</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -748,21 +748,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -772,7 +772,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -782,7 +782,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -792,7 +792,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -802,7 +802,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -812,7 +812,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -822,7 +822,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -832,13 +832,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -876,13 +876,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -898,7 +898,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -932,7 +932,9 @@
         <v>34</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
         <v>41</v>
@@ -962,25 +964,25 @@
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1031,7 +1033,7 @@
         <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H21" t="s">
         <v>42</v>
@@ -1049,14 +1051,14 @@
       <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>52</v>
+      <c r="C23" t="s">
+        <v>88</v>
       </c>
       <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
         <v>57</v>
-      </c>
-      <c r="E23" t="s">
-        <v>58</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
@@ -1095,10 +1097,10 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
         <v>59</v>
-      </c>
-      <c r="E25" t="s">
-        <v>60</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1124,7 +1126,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
@@ -1139,17 +1141,17 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" t="s">
         <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1166,42 +1168,42 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a QuickDisplay method to the TextMenu.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
     <t>Progress</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>ScrollableMenu</t>
+  </si>
+  <si>
+    <t>QuickDisplay()</t>
   </si>
 </sst>
 </file>
@@ -699,10 +702,10 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1083,9 @@
         <v>35</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="4"/>
+      <c r="F24" t="s">
+        <v>89</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
added multiple constructors for the table, rows columns, cells to accept content of type string, MultilineText or object.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -23,6 +23,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alexandru Iuga</author>
+  </authors>
+  <commentList>
+    <comment ref="E20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandru Iuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Close()</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandru Iuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Close()</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandru Iuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Display() / DisplayOnce()</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alexandru Iuga:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+RequestClose()</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
   <si>
@@ -300,7 +406,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +448,19 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -698,14 +817,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1126,7 @@
       <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="1"/>
@@ -1029,7 +1148,7 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F21" t="s">
@@ -1101,10 +1220,10 @@
       <c r="C25" t="s">
         <v>21</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F25" s="1"/>
@@ -1214,5 +1333,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed some methods to match the standard: Spinner.Stop, Prompter.Run, Prompter.RunOnce, Prompter.RequestStop
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -23,114 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Alexandru Iuga</author>
-  </authors>
-  <commentList>
-    <comment ref="E20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandru Iuga:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Close()</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandru Iuga:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Close()</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandru Iuga:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Display() / DisplayOnce()</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E25" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alexandru Iuga:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-RequestClose()</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>Progress</t>
   </si>
@@ -243,12 +137,6 @@
     <t>QuickPause()</t>
   </si>
   <si>
-    <t>Done()</t>
-  </si>
-  <si>
-    <t>Stop()</t>
-  </si>
-  <si>
     <t>Run()</t>
   </si>
   <si>
@@ -306,12 +194,6 @@
     <t>RequestClose()</t>
   </si>
   <si>
-    <t>Run() / RunOnce()</t>
-  </si>
-  <si>
-    <t>RequestStop()</t>
-  </si>
-  <si>
     <t>Play()</t>
   </si>
   <si>
@@ -400,13 +282,16 @@
   </si>
   <si>
     <t>QuickDisplay()</t>
+  </si>
+  <si>
+    <t>Display() / DisplayOnce()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,19 +333,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -817,14 +689,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,34 +704,35 @@
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -870,21 +743,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -894,7 +767,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -904,7 +777,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -914,7 +787,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -924,7 +797,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -934,7 +807,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -944,7 +817,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -954,13 +827,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D11" t="s">
         <v>30</v>
@@ -971,18 +844,18 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -993,18 +866,18 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1015,18 +888,18 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
@@ -1037,7 +910,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1048,7 +921,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
@@ -1059,7 +932,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1070,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -1081,30 +954,30 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -1121,18 +994,18 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>37</v>
+      <c r="E20" t="s">
+        <v>65</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1148,17 +1021,17 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>38</v>
+      <c r="E21" t="s">
+        <v>65</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1174,18 +1047,18 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1203,11 +1076,11 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1220,16 +1093,16 @@
       <c r="C25" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>59</v>
+      <c r="D25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1250,11 +1123,11 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1265,17 +1138,17 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -1292,47 +1165,46 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Table: added methods with params.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Progress</t>
   </si>
@@ -107,15 +107,6 @@
     <t>A class that helps you prevent multiple instances of the same application.</t>
   </si>
   <si>
-    <t>Console MVC Framework</t>
-  </si>
-  <si>
-    <t>A small framework that helps you structure the presentation level of the console application</t>
-  </si>
-  <si>
-    <t>Console MVC</t>
-  </si>
-  <si>
     <t>Read()</t>
   </si>
   <si>
@@ -143,12 +134,6 @@
     <t>Display Mode</t>
   </si>
   <si>
-    <t>Direct read from Console.</t>
-  </si>
-  <si>
-    <t>Direct write to Console.</t>
-  </si>
-  <si>
     <t>Class Name</t>
   </si>
   <si>
@@ -179,15 +164,6 @@
     <t>MachineLevelGuardian</t>
   </si>
   <si>
-    <t>ConsoleApplication</t>
-  </si>
-  <si>
-    <t>Route</t>
-  </si>
-  <si>
-    <t>IController</t>
-  </si>
-  <si>
     <t>Display() / Resume()</t>
   </si>
   <si>
@@ -203,9 +179,6 @@
     <t>Dispose()</t>
   </si>
   <si>
-    <t>Exit()</t>
-  </si>
-  <si>
     <t>Data Read/Write</t>
   </si>
   <si>
@@ -227,9 +200,6 @@
     <t>Dispose Method</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>ITablePrinter</t>
   </si>
   <si>
@@ -285,6 +255,9 @@
   </si>
   <si>
     <t>Display() / DisplayOnce()</t>
+  </si>
+  <si>
+    <t>Direct to Console.</t>
   </si>
 </sst>
 </file>
@@ -690,19 +663,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.7109375" customWidth="1"/>
@@ -712,27 +685,27 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -743,21 +716,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -767,7 +740,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -777,7 +750,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -787,7 +760,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -797,7 +770,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -807,7 +780,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -817,7 +790,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -827,90 +800,90 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,18 +894,18 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -943,41 +916,41 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -994,18 +967,18 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,19 +992,19 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1047,18 +1020,18 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1072,15 +1045,15 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1094,15 +1067,15 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1123,11 +1096,11 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1138,70 +1111,19 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
         <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" t="s">
-        <v>58</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" t="s">
-        <v>67</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified the BorderTemplate class.
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>Progress</t>
   </si>
@@ -107,27 +107,12 @@
     <t>A class that helps you prevent multiple instances of the same application.</t>
   </si>
   <si>
-    <t>Read()</t>
-  </si>
-  <si>
     <t>QuickRead()</t>
   </si>
   <si>
-    <t>Write&lt;T&gt;()</t>
-  </si>
-  <si>
-    <t>QuickWrite&lt;T&gt;()</t>
-  </si>
-  <si>
-    <t>ReadAnswer()</t>
-  </si>
-  <si>
     <t>Display()</t>
   </si>
   <si>
-    <t>QuickPause()</t>
-  </si>
-  <si>
     <t>Run()</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
     <t>ListInput</t>
   </si>
   <si>
-    <t>OutputList</t>
-  </si>
-  <si>
     <t>YesNoQuestion</t>
   </si>
   <si>
@@ -258,6 +240,12 @@
   </si>
   <si>
     <t>HeaderCell / DataGridColumnHeaderCell</t>
+  </si>
+  <si>
+    <t>Display() / ReadAnswer()</t>
+  </si>
+  <si>
+    <t>ListOutput</t>
   </si>
 </sst>
 </file>
@@ -669,7 +657,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,27 +673,27 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -716,21 +704,21 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -740,7 +728,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -750,7 +738,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -760,7 +748,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -770,7 +758,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -780,7 +768,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -790,7 +778,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -800,90 +788,90 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -894,18 +882,18 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -916,41 +904,41 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -967,18 +955,18 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -992,19 +980,19 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="3" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1020,18 +1008,18 @@
         <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1045,15 +1033,15 @@
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1067,15 +1055,15 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1096,11 +1084,11 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1111,17 +1099,17 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H28" s="1"/>
     </row>

</xml_diff>

<commit_message>
#101 - added more tests
</commit_message>
<xml_diff>
--- a/doc/Controls.xlsx
+++ b/doc/Controls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects.pet\ConsoleTools\repo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4D2005-E4E4-4E8C-ADFE-104D8427DEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3F866-3A27-44C6-947E-E63598486D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,30 +256,9 @@
     <t>BackgroundColor</t>
   </si>
   <si>
-    <t>PaddingLeft</t>
-  </si>
-  <si>
-    <t>PaddingRight</t>
-  </si>
-  <si>
-    <t>PaddingTop</t>
-  </si>
-  <si>
-    <t>PaddingBottom</t>
-  </si>
-  <si>
-    <t>HorizontalAlignment</t>
-  </si>
-  <si>
-    <t>VerticalAlignment</t>
-  </si>
-  <si>
     <t>Content</t>
   </si>
   <si>
-    <t>ContentOverflow</t>
-  </si>
-  <si>
     <t>cell</t>
   </si>
   <si>
@@ -298,15 +277,9 @@
     <t>Header</t>
   </si>
   <si>
-    <t>Empty</t>
-  </si>
-  <si>
     <t>Footer</t>
   </si>
   <si>
-    <t>DefaultContent</t>
-  </si>
-  <si>
     <t>ColumnSpan</t>
   </si>
   <si>
@@ -320,6 +293,33 @@
   </si>
   <si>
     <t>Tested</t>
+  </si>
+  <si>
+    <t>CellPaddingLeft</t>
+  </si>
+  <si>
+    <t>CellPaddingRight</t>
+  </si>
+  <si>
+    <t>CellPaddingTop</t>
+  </si>
+  <si>
+    <t>CellPaddingBottom</t>
+  </si>
+  <si>
+    <t>CellHorizontalAlignment</t>
+  </si>
+  <si>
+    <t>CellVerticalAlignment</t>
+  </si>
+  <si>
+    <t>CellDefaultContent</t>
+  </si>
+  <si>
+    <t>CellContentOverflow</t>
+  </si>
+  <si>
+    <t>Empty Grid</t>
   </si>
 </sst>
 </file>
@@ -1262,12 +1262,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U21" sqref="U21"/>
+      <selection pane="topRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" customWidth="1"/>
     <col min="3" max="6" width="12.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="3.85546875" customWidth="1"/>
@@ -1282,31 +1282,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
       <c r="H1" s="10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="M1" s="10" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
       <c r="R1" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="S1" s="10"/>
       <c r="T1" s="10"/>
       <c r="U1" s="10"/>
       <c r="W1" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="X1" s="10"/>
       <c r="Y1" s="10"/>
@@ -1314,64 +1314,64 @@
     </row>
     <row r="2" spans="1:26" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
       <c r="F3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="9"/>
+      <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="7"/>
@@ -1409,7 +1409,7 @@
       <c r="F4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="9"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="7"/>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1476,7 +1476,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="7"/>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="7"/>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="11"/>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1576,32 +1576,32 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
-      <c r="U14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
+      <c r="U14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="7"/>
@@ -1616,7 +1616,7 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="R15" s="11"/>
-      <c r="S15" s="7"/>
+      <c r="S15" s="11"/>
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
       <c r="W15" s="11"/>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
@@ -1652,25 +1652,25 @@
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" s="8"/>
       <c r="D25" s="13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C26" s="12"/>
       <c r="D26" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="13" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
       <c r="D28" s="13" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>